<commit_message>
Added cluster analysis for Halyey
</commit_message>
<xml_diff>
--- a/raw_data/1702KHP-0164_RawData_Stat.xlsx
+++ b/raw_data/1702KHP-0164_RawData_Stat.xlsx
@@ -1044,8 +1044,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="358320d33f278d9b7f7e34366ecf6985">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bd4b1f74759cbf81d0fcc62805ca8ba" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7a124c12a779a736f71215d7d4687bf">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2155876b7947a55992891bc9fceb70da" ns2:_="" ns3:_="">
     <xsd:import namespace="1f3c66e0-7684-4412-85ae-938bcfc42664"/>
     <xsd:import namespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29"/>
     <xsd:element name="properties">
@@ -1067,6 +1067,8 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1135,6 +1137,13 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d7fcee89-5a73-4a7b-ac3d-7e05f09405fb" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" elementFormDefault="qualified">
@@ -1165,6 +1174,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5b0dcb5e-3cf8-47e5-b6b0-eb9332a9b3dc}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="9c30d4e8-d9db-43d6-83e2-c08e4749ca29">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -1279,12 +1299,16 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Flow_SignoffStatus xmlns="1f3c66e0-7684-4412-85ae-938bcfc42664" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f3c66e0-7684-4412-85ae-938bcfc42664">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B130703D-F804-4735-BB0F-4426039B9DA1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{777BE5FE-746F-490E-9C8E-B143FDB218D0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Updated code to align to the published Ar genome
</commit_message>
<xml_diff>
--- a/raw_data/1702KHP-0164_RawData_Stat.xlsx
+++ b/raw_data/1702KHP-0164_RawData_Stat.xlsx
@@ -1044,8 +1044,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7a124c12a779a736f71215d7d4687bf">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2155876b7947a55992891bc9fceb70da" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a115b2da8a2eeee135fdd5733988381">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fe6ebd3e8bf6d9df49fa3e9a691e0f" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="1f3c66e0-7684-4412-85ae-938bcfc42664"/>
     <xsd:import namespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29"/>
     <xsd:element name="properties">
@@ -1069,11 +1070,27 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="24" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="25" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1f3c66e0-7684-4412-85ae-938bcfc42664" elementFormDefault="qualified">
@@ -1303,12 +1320,14 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
     <TaxCatchAll xmlns="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{777BE5FE-746F-490E-9C8E-B143FDB218D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0152C0-49F1-4EF2-898C-3639A420FBAC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Added Octopus and recent FB analysis
</commit_message>
<xml_diff>
--- a/raw_data/1702KHP-0164_RawData_Stat.xlsx
+++ b/raw_data/1702KHP-0164_RawData_Stat.xlsx
@@ -1044,8 +1044,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a115b2da8a2eeee135fdd5733988381">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fe6ebd3e8bf6d9df49fa3e9a691e0f" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="759527f59e11d69b52594aee1565f7b2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfa3fb632320c027112c736c6f89e4dc" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="1f3c66e0-7684-4412-85ae-938bcfc42664"/>
     <xsd:import namespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29"/>
@@ -1072,6 +1072,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1161,6 +1162,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="26" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" elementFormDefault="qualified">
@@ -1327,7 +1333,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0152C0-49F1-4EF2-898C-3639A420FBAC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F622A384-FA54-4182-8429-476E60B40CC1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>